<commit_message>
Redesigned & Improved the patient records modal
</commit_message>
<xml_diff>
--- a/CLASS/SS3/Chemistry/results.xlsx
+++ b/CLASS/SS3/Chemistry/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,49 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Abubakar Fatima Shehu</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>std356</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SS3_GOLD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHEMISTRY</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-12-04 07:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>